<commit_message>
Updated PTBR and CN/TW
</commit_message>
<xml_diff>
--- a/_localisation.xlsx
+++ b/_localisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Projects\Identifile\project-identifile-localisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD800D7-E219-4352-AC9A-58C542FE3F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708E69D4-E5D9-46E7-A82F-CEFBCB0B553A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{DD0ADE5A-0746-48DE-8950-17139D90D8DD}"/>
+    <workbookView xWindow="4890" yWindow="2565" windowWidth="31740" windowHeight="16170" activeTab="1" xr2:uid="{DD0ADE5A-0746-48DE-8950-17139D90D8DD}"/>
   </bookViews>
   <sheets>
     <sheet name="achievements" sheetId="2" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14941" uniqueCount="11998">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15127" uniqueCount="12178">
   <si>
     <t>keys</t>
   </si>
@@ -36396,12 +36396,552 @@
 X Community: 
 @NuraPixel, @_kiseki_miracle, @Lynte_, @m_artstuff, @Duwi_EXE, @Phromn_, @CunnieHoe, @ZeliotL, @trizG_, @NandooPX, @iterateinteract, @gatekid3, @NotMondayGame, @Toadzillart, @NapasGames, @PixelDominus, @TanzDev, @GabreuSenra, @DracoNoko, @Cup_Nooble_, @CursedCode, @Caronte_Caim, @moonlightmae_vt, @auralystic, @Bloopa_Loopa, @SpringloadedDev, @sudonym, @Flashkirby, @w1k3d10, @aintnoking, @HanahoneybeeVT, @Regris_Kallen, @the_polar_pop, @MeanieMoonArt, @jeminix2, @elpichonart, @arsundust, @MiniTankMayhem, @_nyunnya_, @TurtleHolder, @krait181, @lenard_pr, @funa_vt, @_theMatteBlack</t>
   </si>
+  <si>
+    <t>一击识别一个病毒</t>
+  </si>
+  <si>
+    <t>总计识别{x}个正在攻击中的歌姬病毒</t>
+  </si>
+  <si>
+    <t>使用火爆脾气击败复活岛石像</t>
+  </si>
+  <si>
+    <t>通关F盘</t>
+  </si>
+  <si>
+    <t>收集密钥碎片1和2</t>
+  </si>
+  <si>
+    <t>不花费金币的情况下通关</t>
+  </si>
+  <si>
+    <t>捡起 {x} 份文件</t>
+  </si>
+  <si>
+    <t>在木马病毒攻击期间识别出共计 {x} 个木马病毒</t>
+  </si>
+  <si>
+    <t>圆形尾迹</t>
+  </si>
+  <si>
+    <t>三角尾迹</t>
+  </si>
+  <si>
+    <t>星形尾迹</t>
+  </si>
+  <si>
+    <t>硬币尾迹</t>
+  </si>
+  <si>
+    <t>蓝盒尾迹</t>
+  </si>
+  <si>
+    <t>爱心尾迹</t>
+  </si>
+  <si>
+    <t>闪光尾迹</t>
+  </si>
+  <si>
+    <t>光标尾迹</t>
+  </si>
+  <si>
+    <t>呆呆尾迹</t>
+  </si>
+  <si>
+    <t>病毒尾迹</t>
+  </si>
+  <si>
+    <t>太空侵略者尾迹</t>
+  </si>
+  <si>
+    <t>开发者尾迹</t>
+  </si>
+  <si>
+    <t>小夹皮皮肤</t>
+  </si>
+  <si>
+    <t>痞子人生皮肤</t>
+  </si>
+  <si>
+    <t>剑形皮肤</t>
+  </si>
+  <si>
+    <t>镐子皮肤</t>
+  </si>
+  <si>
+    <t>御币皮肤</t>
+  </si>
+  <si>
+    <t>图钉皮肤</t>
+  </si>
+  <si>
+    <t>蓝盒皮肤</t>
+  </si>
+  <si>
+    <t>小鱼皮肤</t>
+  </si>
+  <si>
+    <t>魔法少女皮肤</t>
+  </si>
+  <si>
+    <t>香蕉皮肤</t>
+  </si>
+  <si>
+    <t>披萨皮肤</t>
+  </si>
+  <si>
+    <t>决心皮肤</t>
+  </si>
+  <si>
+    <t>小孢</t>
+  </si>
+  <si>
+    <t>小骷</t>
+  </si>
+  <si>
+    <t>小马</t>
+  </si>
+  <si>
+    <t>小姬</t>
+  </si>
+  <si>
+    <t>压缩炸弹</t>
+  </si>
+  <si>
+    <t>小石</t>
+  </si>
+  <si>
+    <t>阿户</t>
+  </si>
+  <si>
+    <t>小蠕</t>
+  </si>
+  <si>
+    <t>小蛛</t>
+  </si>
+  <si>
+    <t>小卵</t>
+  </si>
+  <si>
+    <t>阿助</t>
+  </si>
+  <si>
+    <t>引导区</t>
+  </si>
+  <si>
+    <t>饼干怪兽</t>
+  </si>
+  <si>
+    <t>伯德</t>
+  </si>
+  <si>
+    <t>小书</t>
+  </si>
+  <si>
+    <t>共匿者</t>
+  </si>
+  <si>
+    <t>震网</t>
+  </si>
+  <si>
+    <t>爆爆</t>
+  </si>
+  <si>
+    <t>蓝精灵</t>
+  </si>
+  <si>
+    <t>阿拉苹果</t>
+  </si>
+  <si>
+    <t>监视者</t>
+  </si>
+  <si>
+    <t>飞马</t>
+  </si>
+  <si>
+    <t>锁位</t>
+  </si>
+  <si>
+    <t>跟套件</t>
+  </si>
+  <si>
+    <t>布谷</t>
+  </si>
+  <si>
+    <t>尼姆达</t>
+  </si>
+  <si>
+    <t>未来</t>
+  </si>
+  <si>
+    <t>萨瑟</t>
+  </si>
+  <si>
+    <t>梅丽莎</t>
+  </si>
+  <si>
+    <t>Z僵尸</t>
+  </si>
+  <si>
+    <t>Bug之祖</t>
+  </si>
+  <si>
+    <t>织网者</t>
+  </si>
+  <si>
+    <t>云核X</t>
+  </si>
+  <si>
+    <t>利维_AI</t>
+  </si>
+  <si>
+    <t>蓝盒</t>
+  </si>
+  <si>
+    <t>迪娜</t>
+  </si>
+  <si>
+    <t>希维亚</t>
+  </si>
+  <si>
+    <t>乔奈</t>
+  </si>
+  <si>
+    <t>首领斗士</t>
+  </si>
+  <si>
+    <t>小兔</t>
+  </si>
+  <si>
+    <t>小古</t>
+  </si>
+  <si>
+    <t>三角头</t>
+  </si>
+  <si>
+    <t>Duwi执行档</t>
+  </si>
+  <si>
+    <t>塞丽娜</t>
+  </si>
+  <si>
+    <t>笑脸</t>
+  </si>
+  <si>
+    <t>坦祖</t>
+  </si>
+  <si>
+    <t>泡沐公主</t>
+  </si>
+  <si>
+    <t>小奇灵</t>
+  </si>
+  <si>
+    <t>美西螈</t>
+  </si>
+  <si>
+    <t>一擊識別一個病毒</t>
+  </si>
+  <si>
+    <t>總計識別{x}個正在攻擊中的歌姬病毒</t>
+  </si>
+  <si>
+    <t>使用火爆脾氣擊敗復活島石像</t>
+  </si>
+  <si>
+    <t>通關F槽</t>
+  </si>
+  <si>
+    <t>收集密鑰碎片1和2</t>
+  </si>
+  <si>
+    <t>在不花費金幣的情況下通關</t>
+  </si>
+  <si>
+    <t>撿起 {x} 份檔案</t>
+  </si>
+  <si>
+    <t>在木馬病毒攻擊期間識別出共計 {x} 個木馬病毒</t>
+  </si>
+  <si>
+    <t>圓形尾跡</t>
+  </si>
+  <si>
+    <t>三角尾跡</t>
+  </si>
+  <si>
+    <t>星形尾跡</t>
+  </si>
+  <si>
+    <t>硬幣尾跡</t>
+  </si>
+  <si>
+    <t>藍盒尾跡</t>
+  </si>
+  <si>
+    <t>愛心尾跡</t>
+  </si>
+  <si>
+    <t>閃光尾跡</t>
+  </si>
+  <si>
+    <t>游標尾跡</t>
+  </si>
+  <si>
+    <t>蠢蠢尾跡</t>
+  </si>
+  <si>
+    <t>病毒尾跡</t>
+  </si>
+  <si>
+    <t>太空侵略者尾跡</t>
+  </si>
+  <si>
+    <t>開發者尾跡</t>
+  </si>
+  <si>
+    <t>小夾皮造型</t>
+  </si>
+  <si>
+    <t>痞子人生造型</t>
+  </si>
+  <si>
+    <t>劍形造型</t>
+  </si>
+  <si>
+    <t>鎬子造型</t>
+  </si>
+  <si>
+    <t>御幣造型</t>
+  </si>
+  <si>
+    <t>圖釘造型</t>
+  </si>
+  <si>
+    <t>藍盒造型</t>
+  </si>
+  <si>
+    <t>魚魚造型</t>
+  </si>
+  <si>
+    <t>魔法少女造型</t>
+  </si>
+  <si>
+    <t>香蕉造型</t>
+  </si>
+  <si>
+    <t>披薩造型</t>
+  </si>
+  <si>
+    <t>決心造型</t>
+  </si>
+  <si>
+    <t>小馬</t>
+  </si>
+  <si>
+    <t>壓縮炸彈</t>
+  </si>
+  <si>
+    <t>阿戶</t>
+  </si>
+  <si>
+    <t>引導區</t>
+  </si>
+  <si>
+    <t>餅乾怪獸</t>
+  </si>
+  <si>
+    <t>小書</t>
+  </si>
+  <si>
+    <t>震網</t>
+  </si>
+  <si>
+    <t>藍精靈</t>
+  </si>
+  <si>
+    <t>阿拉蘋果</t>
+  </si>
+  <si>
+    <t>監視者</t>
+  </si>
+  <si>
+    <t>飛馬</t>
+  </si>
+  <si>
+    <t>鎖位</t>
+  </si>
+  <si>
+    <t>根套件</t>
+  </si>
+  <si>
+    <t>布穀</t>
+  </si>
+  <si>
+    <t>尼姆達</t>
+  </si>
+  <si>
+    <t>未來</t>
+  </si>
+  <si>
+    <t>薩瑟</t>
+  </si>
+  <si>
+    <t>梅麗莎</t>
+  </si>
+  <si>
+    <t>Z殭屍</t>
+  </si>
+  <si>
+    <t>織網者</t>
+  </si>
+  <si>
+    <t>雲核X</t>
+  </si>
+  <si>
+    <t>利維_AI</t>
+  </si>
+  <si>
+    <t>藍盒</t>
+  </si>
+  <si>
+    <t>希維亞</t>
+  </si>
+  <si>
+    <t>喬奈</t>
+  </si>
+  <si>
+    <t>首領鬥士</t>
+  </si>
+  <si>
+    <t>三角頭</t>
+  </si>
+  <si>
+    <t>Duwi執行檔</t>
+  </si>
+  <si>
+    <t>塞麗娜</t>
+  </si>
+  <si>
+    <t>笑臉</t>
+  </si>
+  <si>
+    <t>小奇靈</t>
+  </si>
+  <si>
+    <t>美西鯰</t>
+  </si>
+  <si>
+    <t>致命尖刺</t>
+  </si>
+  <si>
+    <t>病毒死亡时会射出尖刺</t>
+  </si>
+  <si>
+    <t>尸爆术</t>
+  </si>
+  <si>
+    <t>病毒死亡后会在短暂延迟后爆炸</t>
+  </si>
+  <si>
+    <t>吸血之触</t>
+  </si>
+  <si>
+    <t>病毒攻击命中玩家后会回复生命值</t>
+  </si>
+  <si>
+    <t>兜不住啦</t>
+  </si>
+  <si>
+    <t>受到伤害时有几率掉落金币</t>
+  </si>
+  <si>
+    <t>强化病毒</t>
+  </si>
+  <si>
+    <t>病毒有几率以增加 {x}% 生命值的状态生成</t>
+  </si>
+  <si>
+    <t>病毒变异</t>
+  </si>
+  <si>
+    <t>病毒有几率生成时带有随机强化效果</t>
+  </si>
+  <si>
+    <t>人固有一死</t>
+  </si>
+  <si>
+    <t>玩家受到任何伤害都会直接死亡</t>
+  </si>
+  <si>
+    <t>病毒增援</t>
+  </si>
+  <si>
+    <t>病毒死亡后有几率重新生成</t>
+  </si>
+  <si>
+    <t>搏一搏，单车变摩托</t>
+  </si>
+  <si>
+    <t>玩家造成与承受的伤害都会提升 {x} 倍</t>
+  </si>
+  <si>
+    <t>病毒再生</t>
+  </si>
+  <si>
+    <t>病毒会随时间逐渐恢复生命值</t>
+  </si>
+  <si>
+    <t>病毒死亡時會射出尖刺</t>
+  </si>
+  <si>
+    <t>屍爆術</t>
+  </si>
+  <si>
+    <t>病毒死亡後會在短暫延遲後爆炸</t>
+  </si>
+  <si>
+    <t>吸血之觸</t>
+  </si>
+  <si>
+    <t>病毒攻擊命中玩家後會回復生命值</t>
+  </si>
+  <si>
+    <t>受到傷害時有機率掉落金幣</t>
+  </si>
+  <si>
+    <t>強化病毒</t>
+  </si>
+  <si>
+    <t>病毒有機率以增加 {x}% 生命值的狀態生成</t>
+  </si>
+  <si>
+    <t>病毒變異</t>
+  </si>
+  <si>
+    <t>病毒有機率生成時帶有隨機強化效果</t>
+  </si>
+  <si>
+    <t>玩家受到任何傷害都會直接死亡</t>
+  </si>
+  <si>
+    <t>病毒死亡後有機率重新生成</t>
+  </si>
+  <si>
+    <t>搏一搏，單車變摩托</t>
+  </si>
+  <si>
+    <t>玩家造成與承受的傷害都會提升 {x} 倍</t>
+  </si>
+  <si>
+    <t>病毒會隨時間逐漸恢復生命值</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -36465,6 +37005,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -36485,7 +37031,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -36508,6 +37054,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -36518,7 +37079,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -36535,6 +37096,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -37862,7 +38427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3EBBEE6-3641-47DF-A45B-B07C4C2D09D6}">
   <dimension ref="A1:O204"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
+    <sheetView topLeftCell="A145" workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
@@ -43718,7 +44283,7 @@
   <dimension ref="A1:O223"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43783,6 +44348,12 @@
       <c r="C2" t="s">
         <v>7384</v>
       </c>
+      <c r="D2" t="s">
+        <v>12143</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12143</v>
+      </c>
       <c r="F2" s="6" t="s">
         <v>6907</v>
       </c>
@@ -43812,6 +44383,12 @@
       <c r="C3" t="s">
         <v>7385</v>
       </c>
+      <c r="D3" t="s">
+        <v>12144</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12163</v>
+      </c>
       <c r="F3" s="6" t="s">
         <v>6908</v>
       </c>
@@ -43841,6 +44418,12 @@
       <c r="C4" t="s">
         <v>7386</v>
       </c>
+      <c r="D4" t="s">
+        <v>12145</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12164</v>
+      </c>
       <c r="F4" s="6" t="s">
         <v>6909</v>
       </c>
@@ -43870,6 +44453,12 @@
       <c r="C5" t="s">
         <v>7387</v>
       </c>
+      <c r="D5" t="s">
+        <v>12146</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12165</v>
+      </c>
       <c r="F5" s="6" t="s">
         <v>6910</v>
       </c>
@@ -43899,6 +44488,12 @@
       <c r="C6" t="s">
         <v>7388</v>
       </c>
+      <c r="D6" t="s">
+        <v>12147</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12166</v>
+      </c>
       <c r="F6" s="6" t="s">
         <v>6911</v>
       </c>
@@ -43928,6 +44523,12 @@
       <c r="C7" t="s">
         <v>7389</v>
       </c>
+      <c r="D7" t="s">
+        <v>12148</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12167</v>
+      </c>
       <c r="F7" s="6" t="s">
         <v>6912</v>
       </c>
@@ -43957,6 +44558,12 @@
       <c r="C8" t="s">
         <v>7390</v>
       </c>
+      <c r="D8" t="s">
+        <v>12149</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12149</v>
+      </c>
       <c r="F8" s="6" t="s">
         <v>6913</v>
       </c>
@@ -43986,6 +44593,12 @@
       <c r="C9" t="s">
         <v>7391</v>
       </c>
+      <c r="D9" t="s">
+        <v>12150</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12168</v>
+      </c>
       <c r="F9" s="6" t="s">
         <v>6914</v>
       </c>
@@ -44015,6 +44628,12 @@
       <c r="C10" t="s">
         <v>7392</v>
       </c>
+      <c r="D10" t="s">
+        <v>12151</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12169</v>
+      </c>
       <c r="F10" s="6" t="s">
         <v>6915</v>
       </c>
@@ -44044,6 +44663,12 @@
       <c r="C11" t="s">
         <v>7393</v>
       </c>
+      <c r="D11" t="s">
+        <v>12152</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12170</v>
+      </c>
       <c r="F11" s="6" t="s">
         <v>6916</v>
       </c>
@@ -44073,6 +44698,12 @@
       <c r="C12" t="s">
         <v>7394</v>
       </c>
+      <c r="D12" t="s">
+        <v>12153</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12171</v>
+      </c>
       <c r="F12" s="6" t="s">
         <v>6917</v>
       </c>
@@ -44102,6 +44733,12 @@
       <c r="C13" t="s">
         <v>7395</v>
       </c>
+      <c r="D13" t="s">
+        <v>12154</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12172</v>
+      </c>
       <c r="F13" s="6" t="s">
         <v>6918</v>
       </c>
@@ -44131,6 +44768,12 @@
       <c r="C14" t="s">
         <v>7396</v>
       </c>
+      <c r="D14" t="s">
+        <v>12155</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12155</v>
+      </c>
       <c r="F14" s="6" t="s">
         <v>5728</v>
       </c>
@@ -44160,6 +44803,12 @@
       <c r="C15" t="s">
         <v>7397</v>
       </c>
+      <c r="D15" t="s">
+        <v>12156</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12173</v>
+      </c>
       <c r="F15" s="6" t="s">
         <v>6919</v>
       </c>
@@ -44190,10 +44839,10 @@
         <v>6287</v>
       </c>
       <c r="D16" t="s">
-        <v>6287</v>
+        <v>12153</v>
       </c>
       <c r="E16" t="s">
-        <v>6287</v>
+        <v>12171</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>6287</v>
@@ -44237,10 +44886,10 @@
         <v>6287</v>
       </c>
       <c r="D17" t="s">
-        <v>6287</v>
+        <v>12154</v>
       </c>
       <c r="E17" t="s">
-        <v>6287</v>
+        <v>12172</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>6287</v>
@@ -44283,6 +44932,12 @@
       <c r="C18" t="s">
         <v>7398</v>
       </c>
+      <c r="D18" t="s">
+        <v>12157</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12157</v>
+      </c>
       <c r="F18" s="6" t="s">
         <v>6920</v>
       </c>
@@ -44312,6 +44967,12 @@
       <c r="C19" t="s">
         <v>7399</v>
       </c>
+      <c r="D19" t="s">
+        <v>12158</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12174</v>
+      </c>
       <c r="F19" s="6" t="s">
         <v>6921</v>
       </c>
@@ -44341,6 +45002,12 @@
       <c r="C20" t="s">
         <v>7400</v>
       </c>
+      <c r="D20" t="s">
+        <v>12159</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12175</v>
+      </c>
       <c r="F20" s="6" t="s">
         <v>6922</v>
       </c>
@@ -44370,6 +45037,12 @@
       <c r="C21" t="s">
         <v>7401</v>
       </c>
+      <c r="D21" t="s">
+        <v>12160</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12176</v>
+      </c>
       <c r="F21" s="6" t="s">
         <v>6923</v>
       </c>
@@ -44399,6 +45072,12 @@
       <c r="C22" t="s">
         <v>7402</v>
       </c>
+      <c r="D22" t="s">
+        <v>12161</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12161</v>
+      </c>
       <c r="F22" s="6" t="s">
         <v>6924</v>
       </c>
@@ -44428,6 +45107,12 @@
       <c r="C23" t="s">
         <v>7403</v>
       </c>
+      <c r="D23" t="s">
+        <v>12162</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12177</v>
+      </c>
       <c r="F23" s="6" t="s">
         <v>6925</v>
       </c>
@@ -44714,244 +45399,360 @@
     <row r="112" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F112" s="2"/>
     </row>
-    <row r="113" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F113" s="2"/>
     </row>
-    <row r="114" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D114" s="10"/>
+      <c r="E114" s="10"/>
       <c r="F114" s="2"/>
     </row>
-    <row r="115" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F115" s="2"/>
     </row>
-    <row r="116" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F116" s="2"/>
     </row>
-    <row r="117" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F117" s="2"/>
     </row>
-    <row r="118" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F118" s="2"/>
     </row>
-    <row r="119" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F119" s="2"/>
     </row>
-    <row r="120" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D120" s="10"/>
+      <c r="E120" s="10"/>
       <c r="F120" s="2"/>
     </row>
-    <row r="121" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F121" s="2"/>
     </row>
-    <row r="122" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D122" s="10"/>
+      <c r="E122" s="10"/>
       <c r="F122" s="2"/>
     </row>
-    <row r="123" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F123" s="2"/>
     </row>
-    <row r="124" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F124" s="2"/>
     </row>
-    <row r="125" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F125" s="2"/>
     </row>
-    <row r="126" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F126" s="2"/>
     </row>
-    <row r="127" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F127" s="2"/>
     </row>
-    <row r="128" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F128" s="2"/>
     </row>
-    <row r="129" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F129" s="2"/>
     </row>
-    <row r="130" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F130" s="2"/>
     </row>
-    <row r="131" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F131" s="2"/>
     </row>
-    <row r="132" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F132" s="2"/>
     </row>
-    <row r="133" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F133" s="2"/>
     </row>
-    <row r="134" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F134" s="2"/>
     </row>
-    <row r="135" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D135" s="13"/>
+      <c r="E135" s="13"/>
       <c r="F135" s="5"/>
     </row>
-    <row r="136" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D136" s="13"/>
+      <c r="E136" s="13"/>
       <c r="F136" s="5"/>
     </row>
-    <row r="137" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D137" s="13"/>
+      <c r="E137" s="13"/>
       <c r="F137" s="5"/>
     </row>
-    <row r="138" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D138" s="13"/>
+      <c r="E138" s="13"/>
       <c r="F138" s="5"/>
     </row>
-    <row r="139" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D139" s="13"/>
+      <c r="E139" s="13"/>
       <c r="F139" s="5"/>
     </row>
-    <row r="140" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D140" s="13"/>
+      <c r="E140" s="13"/>
       <c r="F140" s="5"/>
     </row>
-    <row r="141" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D141" s="13"/>
+      <c r="E141" s="13"/>
       <c r="F141" s="5"/>
     </row>
-    <row r="142" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D142" s="13"/>
+      <c r="E142" s="13"/>
       <c r="F142" s="5"/>
     </row>
-    <row r="143" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D143" s="13"/>
+      <c r="E143" s="13"/>
       <c r="F143" s="5"/>
     </row>
-    <row r="144" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D144" s="13"/>
+      <c r="E144" s="13"/>
       <c r="F144" s="5"/>
     </row>
-    <row r="145" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D145" s="13"/>
+      <c r="E145" s="13"/>
       <c r="F145" s="5"/>
     </row>
-    <row r="146" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D146" s="13"/>
+      <c r="E146" s="13"/>
       <c r="F146" s="5"/>
     </row>
-    <row r="147" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D147" s="13"/>
+      <c r="E147" s="13"/>
       <c r="F147" s="5"/>
     </row>
-    <row r="148" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D148" s="13"/>
+      <c r="E148" s="13"/>
       <c r="F148" s="5"/>
     </row>
-    <row r="149" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D149" s="13"/>
+      <c r="E149" s="13"/>
       <c r="F149" s="5"/>
     </row>
-    <row r="150" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D150" s="13"/>
+      <c r="E150" s="13"/>
       <c r="F150" s="5"/>
     </row>
-    <row r="151" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D151" s="13"/>
+      <c r="E151" s="13"/>
       <c r="F151" s="5"/>
     </row>
-    <row r="152" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D152" s="13"/>
+      <c r="E152" s="13"/>
       <c r="F152" s="5"/>
     </row>
-    <row r="153" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D153" s="13"/>
+      <c r="E153" s="13"/>
       <c r="F153" s="5"/>
     </row>
-    <row r="154" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D154" s="13"/>
+      <c r="E154" s="13"/>
       <c r="F154" s="5"/>
     </row>
-    <row r="155" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D155" s="13"/>
+      <c r="E155" s="13"/>
       <c r="F155" s="5"/>
     </row>
-    <row r="156" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D156" s="13"/>
+      <c r="E156" s="13"/>
       <c r="F156" s="5"/>
     </row>
-    <row r="157" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D157" s="13"/>
+      <c r="E157" s="13"/>
       <c r="F157" s="5"/>
     </row>
-    <row r="158" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D158" s="13"/>
+      <c r="E158" s="13"/>
       <c r="F158" s="5"/>
     </row>
-    <row r="159" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D159" s="13"/>
+      <c r="E159" s="13"/>
       <c r="F159" s="5"/>
     </row>
-    <row r="160" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D160" s="10"/>
+      <c r="E160" s="10"/>
       <c r="F160" s="5"/>
     </row>
-    <row r="161" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D161" s="10"/>
+      <c r="E161" s="10"/>
       <c r="F161" s="5"/>
     </row>
-    <row r="162" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D162" s="10"/>
+      <c r="E162" s="10"/>
       <c r="F162" s="5"/>
     </row>
-    <row r="163" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D163" s="10"/>
+      <c r="E163" s="10"/>
       <c r="F163" s="5"/>
     </row>
-    <row r="164" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D164" s="10"/>
+      <c r="E164" s="10"/>
       <c r="F164" s="5"/>
     </row>
-    <row r="165" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D165" s="10"/>
+      <c r="E165" s="10"/>
       <c r="F165" s="5"/>
     </row>
-    <row r="166" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D166" s="10"/>
+      <c r="E166" s="10"/>
       <c r="F166" s="5"/>
     </row>
-    <row r="167" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D167" s="10"/>
+      <c r="E167" s="10"/>
       <c r="F167" s="5"/>
     </row>
-    <row r="168" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D168" s="10"/>
+      <c r="E168" s="10"/>
       <c r="F168" s="5"/>
     </row>
-    <row r="169" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D169" s="10"/>
+      <c r="E169" s="10"/>
       <c r="F169" s="5"/>
     </row>
-    <row r="170" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D170" s="10"/>
+      <c r="E170" s="10"/>
       <c r="F170" s="5"/>
     </row>
-    <row r="171" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D171" s="10"/>
+      <c r="E171" s="10"/>
       <c r="F171" s="5"/>
     </row>
-    <row r="172" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D172" s="10"/>
+      <c r="E172" s="10"/>
       <c r="F172" s="5"/>
     </row>
-    <row r="173" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D173" s="10"/>
+      <c r="E173" s="10"/>
       <c r="F173" s="5"/>
     </row>
-    <row r="174" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D174" s="10"/>
+      <c r="E174" s="10"/>
       <c r="F174" s="5"/>
     </row>
-    <row r="175" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D175" s="10"/>
+      <c r="E175" s="10"/>
       <c r="F175" s="5"/>
     </row>
-    <row r="176" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D176" s="10"/>
+      <c r="E176" s="10"/>
       <c r="F176" s="5"/>
     </row>
-    <row r="177" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D177" s="10"/>
+      <c r="E177" s="10"/>
       <c r="F177" s="5"/>
     </row>
-    <row r="178" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D178" s="10"/>
+      <c r="E178" s="10"/>
       <c r="F178" s="5"/>
     </row>
-    <row r="179" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D179" s="10"/>
+      <c r="E179" s="10"/>
       <c r="F179" s="5"/>
     </row>
-    <row r="180" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D180" s="10"/>
+      <c r="E180" s="10"/>
       <c r="F180" s="5"/>
     </row>
-    <row r="181" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D181" s="10"/>
+      <c r="E181" s="10"/>
       <c r="F181" s="5"/>
     </row>
-    <row r="182" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D182" s="10"/>
+      <c r="E182" s="10"/>
       <c r="F182" s="5"/>
     </row>
-    <row r="183" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D183" s="10"/>
+      <c r="E183" s="10"/>
       <c r="F183" s="5"/>
     </row>
-    <row r="184" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D184" s="10"/>
+      <c r="E184" s="10"/>
       <c r="F184" s="5"/>
     </row>
-    <row r="185" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D185" s="10"/>
+      <c r="E185" s="10"/>
       <c r="F185" s="5"/>
     </row>
-    <row r="186" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D186" s="10"/>
+      <c r="E186" s="10"/>
       <c r="F186" s="5"/>
     </row>
-    <row r="187" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D187" s="10"/>
+      <c r="E187" s="10"/>
       <c r="F187" s="5"/>
     </row>
-    <row r="188" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D188" s="10"/>
+      <c r="E188" s="10"/>
       <c r="F188" s="5"/>
     </row>
-    <row r="189" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D189" s="10"/>
+      <c r="E189" s="10"/>
       <c r="F189" s="5"/>
     </row>
-    <row r="190" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F190" s="6"/>
     </row>
-    <row r="191" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F191" s="6"/>
     </row>
-    <row r="192" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="4:6" x14ac:dyDescent="0.25">
       <c r="F192" s="6"/>
     </row>
     <row r="193" spans="6:6" x14ac:dyDescent="0.25">
@@ -45060,8 +45861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58FBDDAB-2921-4157-8A97-8D71EE2B7C38}">
   <dimension ref="A1:O255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="E46" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47631,8 +48432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54479BFB-F3D2-4D17-B932-698CB7EE6AC8}">
   <dimension ref="A1:O323"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G146" sqref="G146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48187,11 +48988,11 @@
       <c r="C16" t="s">
         <v>7114</v>
       </c>
-      <c r="D16" t="s">
-        <v>4481</v>
-      </c>
-      <c r="E16" t="s">
-        <v>4482</v>
+      <c r="D16" s="10" t="s">
+        <v>11998</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>12079</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>6753</v>
@@ -48257,10 +49058,10 @@
       <c r="C18" t="s">
         <v>7116</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="10" t="s">
         <v>5328</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="10" t="s">
         <v>5329</v>
       </c>
       <c r="F18" s="5" t="s">
@@ -48292,11 +49093,11 @@
       <c r="C19" t="s">
         <v>7117</v>
       </c>
-      <c r="D19" t="s">
-        <v>4481</v>
-      </c>
-      <c r="E19" t="s">
-        <v>4482</v>
+      <c r="D19" s="10" t="s">
+        <v>11999</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>12080</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>6790</v>
@@ -48362,10 +49163,10 @@
       <c r="C21" t="s">
         <v>7119</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="10" t="s">
         <v>5332</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="10" t="s">
         <v>5333</v>
       </c>
       <c r="F21" s="5" t="s">
@@ -48397,11 +49198,11 @@
       <c r="C22" t="s">
         <v>7120</v>
       </c>
-      <c r="D22" t="s">
-        <v>4481</v>
-      </c>
-      <c r="E22" t="s">
-        <v>4482</v>
+      <c r="D22" s="10" t="s">
+        <v>12000</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>12081</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>6792</v>
@@ -48502,11 +49303,11 @@
       <c r="C25" t="s">
         <v>7123</v>
       </c>
-      <c r="D25" t="s">
-        <v>4481</v>
-      </c>
-      <c r="E25" t="s">
-        <v>4482</v>
+      <c r="D25" s="10" t="s">
+        <v>12001</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>12082</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>6793</v>
@@ -48607,11 +49408,11 @@
       <c r="C28" t="s">
         <v>7126</v>
       </c>
-      <c r="D28" t="s">
-        <v>4481</v>
-      </c>
-      <c r="E28" t="s">
-        <v>4482</v>
+      <c r="D28" s="10" t="s">
+        <v>12002</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>12083</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>6795</v>
@@ -48712,11 +49513,11 @@
       <c r="C31" t="s">
         <v>7129</v>
       </c>
-      <c r="D31" t="s">
-        <v>4481</v>
-      </c>
-      <c r="E31" t="s">
-        <v>4482</v>
+      <c r="D31" s="10" t="s">
+        <v>12003</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>12084</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>6796</v>
@@ -48817,11 +49618,11 @@
       <c r="C34" t="s">
         <v>7132</v>
       </c>
-      <c r="D34" t="s">
-        <v>4481</v>
-      </c>
-      <c r="E34" t="s">
-        <v>4482</v>
+      <c r="D34" s="10" t="s">
+        <v>12004</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>12085</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>6797</v>
@@ -48922,11 +49723,11 @@
       <c r="C37" t="s">
         <v>7135</v>
       </c>
-      <c r="D37" t="s">
-        <v>4481</v>
-      </c>
-      <c r="E37" t="s">
-        <v>4482</v>
+      <c r="D37" s="10" t="s">
+        <v>12005</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>12086</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>6798</v>
@@ -48957,10 +49758,10 @@
       <c r="C38" t="s">
         <v>7136</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="10" t="s">
         <v>5354</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="10" t="s">
         <v>5355</v>
       </c>
       <c r="F38" s="5" t="s">
@@ -48992,10 +49793,10 @@
       <c r="C39" t="s">
         <v>7137</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="10" t="s">
         <v>4561</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="10" t="s">
         <v>4562</v>
       </c>
       <c r="F39" s="5" t="s">
@@ -49027,10 +49828,10 @@
       <c r="C40" t="s">
         <v>7137</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="10" t="s">
         <v>4561</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="10" t="s">
         <v>4562</v>
       </c>
       <c r="F40" s="5" t="s">
@@ -49062,10 +49863,10 @@
       <c r="C41" t="s">
         <v>7138</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="10" t="s">
         <v>5356</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="10" t="s">
         <v>5357</v>
       </c>
       <c r="F41" s="5" t="s">
@@ -49097,10 +49898,10 @@
       <c r="C42" t="s">
         <v>7137</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="10" t="s">
         <v>4561</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="10" t="s">
         <v>4562</v>
       </c>
       <c r="F42" s="5" t="s">
@@ -49132,10 +49933,10 @@
       <c r="C43" t="s">
         <v>7137</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="10" t="s">
         <v>4561</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="10" t="s">
         <v>4562</v>
       </c>
       <c r="F43" s="5" t="s">
@@ -49167,10 +49968,10 @@
       <c r="C44" t="s">
         <v>7139</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="10" t="s">
         <v>5358</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="10" t="s">
         <v>5359</v>
       </c>
       <c r="F44" s="5" t="s">
@@ -49202,10 +50003,10 @@
       <c r="C45" t="s">
         <v>7137</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="10" t="s">
         <v>4561</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="10" t="s">
         <v>4562</v>
       </c>
       <c r="F45" s="5" t="s">
@@ -49237,10 +50038,10 @@
       <c r="C46" t="s">
         <v>7137</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="10" t="s">
         <v>4561</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="10" t="s">
         <v>4562</v>
       </c>
       <c r="F46" s="5" t="s">
@@ -49348,6 +50149,12 @@
       <c r="C50" t="s">
         <v>7141</v>
       </c>
+      <c r="D50" t="s">
+        <v>12006</v>
+      </c>
+      <c r="E50" t="s">
+        <v>12087</v>
+      </c>
       <c r="F50" s="2" t="s">
         <v>6799</v>
       </c>
@@ -49377,6 +50184,12 @@
       <c r="C51" t="s">
         <v>7142</v>
       </c>
+      <c r="D51" t="s">
+        <v>12007</v>
+      </c>
+      <c r="E51" t="s">
+        <v>12088</v>
+      </c>
       <c r="F51" s="2" t="s">
         <v>6800</v>
       </c>
@@ -49406,6 +50219,12 @@
       <c r="C52" t="s">
         <v>7143</v>
       </c>
+      <c r="D52" t="s">
+        <v>12008</v>
+      </c>
+      <c r="E52" t="s">
+        <v>12089</v>
+      </c>
       <c r="F52" s="2" t="s">
         <v>6801</v>
       </c>
@@ -49435,6 +50254,12 @@
       <c r="C53" t="s">
         <v>7144</v>
       </c>
+      <c r="D53" t="s">
+        <v>12009</v>
+      </c>
+      <c r="E53" t="s">
+        <v>12090</v>
+      </c>
       <c r="F53" s="2" t="s">
         <v>6802</v>
       </c>
@@ -49464,6 +50289,12 @@
       <c r="C54" t="s">
         <v>7145</v>
       </c>
+      <c r="D54" t="s">
+        <v>12010</v>
+      </c>
+      <c r="E54" t="s">
+        <v>12091</v>
+      </c>
       <c r="F54" s="2" t="s">
         <v>6803</v>
       </c>
@@ -49493,6 +50324,12 @@
       <c r="C55" t="s">
         <v>7146</v>
       </c>
+      <c r="D55" t="s">
+        <v>12011</v>
+      </c>
+      <c r="E55" t="s">
+        <v>12092</v>
+      </c>
       <c r="F55" s="2" t="s">
         <v>6804</v>
       </c>
@@ -49522,6 +50359,12 @@
       <c r="C56" t="s">
         <v>7147</v>
       </c>
+      <c r="D56" t="s">
+        <v>12012</v>
+      </c>
+      <c r="E56" t="s">
+        <v>12093</v>
+      </c>
       <c r="F56" s="2" t="s">
         <v>6805</v>
       </c>
@@ -49551,6 +50394,12 @@
       <c r="C57" t="s">
         <v>7148</v>
       </c>
+      <c r="D57" t="s">
+        <v>12013</v>
+      </c>
+      <c r="E57" t="s">
+        <v>12094</v>
+      </c>
       <c r="F57" s="2" t="s">
         <v>6806</v>
       </c>
@@ -49580,6 +50429,12 @@
       <c r="C58" t="s">
         <v>7149</v>
       </c>
+      <c r="D58" t="s">
+        <v>12014</v>
+      </c>
+      <c r="E58" t="s">
+        <v>12095</v>
+      </c>
       <c r="F58" s="2" t="s">
         <v>6807</v>
       </c>
@@ -49609,6 +50464,12 @@
       <c r="C59" t="s">
         <v>7150</v>
       </c>
+      <c r="D59" t="s">
+        <v>12015</v>
+      </c>
+      <c r="E59" t="s">
+        <v>12096</v>
+      </c>
       <c r="F59" s="2" t="s">
         <v>6808</v>
       </c>
@@ -49638,6 +50499,12 @@
       <c r="C60" t="s">
         <v>7151</v>
       </c>
+      <c r="D60" t="s">
+        <v>12016</v>
+      </c>
+      <c r="E60" t="s">
+        <v>12097</v>
+      </c>
       <c r="F60" s="2" t="s">
         <v>6192</v>
       </c>
@@ -49667,6 +50534,12 @@
       <c r="C61" t="s">
         <v>7152</v>
       </c>
+      <c r="D61" t="s">
+        <v>12017</v>
+      </c>
+      <c r="E61" t="s">
+        <v>12098</v>
+      </c>
       <c r="F61" s="2" t="s">
         <v>6809</v>
       </c>
@@ -49702,6 +50575,12 @@
       <c r="C63" t="s">
         <v>7153</v>
       </c>
+      <c r="D63" t="s">
+        <v>12018</v>
+      </c>
+      <c r="E63" t="s">
+        <v>12099</v>
+      </c>
       <c r="F63" s="2" t="s">
         <v>6810</v>
       </c>
@@ -49731,6 +50610,12 @@
       <c r="C64" t="s">
         <v>7154</v>
       </c>
+      <c r="D64" t="s">
+        <v>12019</v>
+      </c>
+      <c r="E64" t="s">
+        <v>12100</v>
+      </c>
       <c r="F64" s="2" t="s">
         <v>6811</v>
       </c>
@@ -49760,6 +50645,12 @@
       <c r="C65" t="s">
         <v>7155</v>
       </c>
+      <c r="D65" t="s">
+        <v>12020</v>
+      </c>
+      <c r="E65" t="s">
+        <v>12101</v>
+      </c>
       <c r="F65" s="2" t="s">
         <v>6812</v>
       </c>
@@ -49789,6 +50680,12 @@
       <c r="C66" t="s">
         <v>7156</v>
       </c>
+      <c r="D66" t="s">
+        <v>12021</v>
+      </c>
+      <c r="E66" t="s">
+        <v>12102</v>
+      </c>
       <c r="F66" s="2" t="s">
         <v>6813</v>
       </c>
@@ -49818,6 +50715,12 @@
       <c r="C67" t="s">
         <v>7157</v>
       </c>
+      <c r="D67" t="s">
+        <v>12022</v>
+      </c>
+      <c r="E67" t="s">
+        <v>12103</v>
+      </c>
       <c r="F67" s="2" t="s">
         <v>6814</v>
       </c>
@@ -49847,6 +50750,12 @@
       <c r="C68" t="s">
         <v>7158</v>
       </c>
+      <c r="D68" t="s">
+        <v>12023</v>
+      </c>
+      <c r="E68" t="s">
+        <v>12104</v>
+      </c>
       <c r="F68" s="2" t="s">
         <v>6815</v>
       </c>
@@ -49876,6 +50785,12 @@
       <c r="C69" t="s">
         <v>7159</v>
       </c>
+      <c r="D69" t="s">
+        <v>12024</v>
+      </c>
+      <c r="E69" t="s">
+        <v>12105</v>
+      </c>
       <c r="F69" s="2" t="s">
         <v>6816</v>
       </c>
@@ -49905,6 +50820,12 @@
       <c r="C70" t="s">
         <v>7160</v>
       </c>
+      <c r="D70" t="s">
+        <v>12025</v>
+      </c>
+      <c r="E70" t="s">
+        <v>12106</v>
+      </c>
       <c r="F70" s="2" t="s">
         <v>6817</v>
       </c>
@@ -49934,6 +50855,12 @@
       <c r="C71" t="s">
         <v>7161</v>
       </c>
+      <c r="D71" t="s">
+        <v>12026</v>
+      </c>
+      <c r="E71" t="s">
+        <v>12107</v>
+      </c>
       <c r="F71" s="2" t="s">
         <v>6818</v>
       </c>
@@ -49963,6 +50890,12 @@
       <c r="C72" t="s">
         <v>7162</v>
       </c>
+      <c r="D72" t="s">
+        <v>12027</v>
+      </c>
+      <c r="E72" t="s">
+        <v>12108</v>
+      </c>
       <c r="F72" s="2" t="s">
         <v>6819</v>
       </c>
@@ -49992,6 +50925,12 @@
       <c r="C73" t="s">
         <v>7163</v>
       </c>
+      <c r="D73" t="s">
+        <v>12028</v>
+      </c>
+      <c r="E73" t="s">
+        <v>12109</v>
+      </c>
       <c r="F73" s="2" t="s">
         <v>6820</v>
       </c>
@@ -50011,7 +50950,7 @@
         <v>11479</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>5801</v>
       </c>
@@ -50021,6 +50960,12 @@
       <c r="C74" t="s">
         <v>7164</v>
       </c>
+      <c r="D74" t="s">
+        <v>12029</v>
+      </c>
+      <c r="E74" t="s">
+        <v>12110</v>
+      </c>
       <c r="F74" s="2" t="s">
         <v>6821</v>
       </c>
@@ -50040,7 +50985,7 @@
         <v>6205</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>5803</v>
       </c>
@@ -50050,6 +50995,12 @@
       <c r="C75" t="s">
         <v>7165</v>
       </c>
+      <c r="D75" s="12" t="s">
+        <v>12030</v>
+      </c>
+      <c r="E75" s="12" t="s">
+        <v>12030</v>
+      </c>
       <c r="F75" s="2" t="s">
         <v>6822</v>
       </c>
@@ -50069,7 +51020,7 @@
         <v>6206</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>5805</v>
       </c>
@@ -50079,6 +51030,12 @@
       <c r="C76" t="s">
         <v>7166</v>
       </c>
+      <c r="D76" s="12" t="s">
+        <v>12031</v>
+      </c>
+      <c r="E76" s="12" t="s">
+        <v>12031</v>
+      </c>
       <c r="F76" s="2" t="s">
         <v>6823</v>
       </c>
@@ -50098,7 +51055,7 @@
         <v>6207</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>5807</v>
       </c>
@@ -50108,6 +51065,12 @@
       <c r="C77" t="s">
         <v>7167</v>
       </c>
+      <c r="D77" s="12" t="s">
+        <v>12032</v>
+      </c>
+      <c r="E77" s="12" t="s">
+        <v>12111</v>
+      </c>
       <c r="F77" s="2" t="s">
         <v>5808</v>
       </c>
@@ -50127,7 +51090,7 @@
         <v>6208</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>5809</v>
       </c>
@@ -50137,6 +51100,12 @@
       <c r="C78" t="s">
         <v>7168</v>
       </c>
+      <c r="D78" s="12" t="s">
+        <v>12033</v>
+      </c>
+      <c r="E78" s="12" t="s">
+        <v>12033</v>
+      </c>
       <c r="F78" s="2" t="s">
         <v>5810</v>
       </c>
@@ -50156,7 +51125,7 @@
         <v>5810</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>5811</v>
       </c>
@@ -50166,6 +51135,12 @@
       <c r="C79" t="s">
         <v>7169</v>
       </c>
+      <c r="D79" s="12" t="s">
+        <v>12034</v>
+      </c>
+      <c r="E79" s="12" t="s">
+        <v>12112</v>
+      </c>
       <c r="F79" s="2" t="s">
         <v>5812</v>
       </c>
@@ -50185,7 +51160,7 @@
         <v>11480</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>5813</v>
       </c>
@@ -50195,6 +51170,12 @@
       <c r="C80" t="s">
         <v>7170</v>
       </c>
+      <c r="D80" s="12" t="s">
+        <v>12035</v>
+      </c>
+      <c r="E80" s="12" t="s">
+        <v>12035</v>
+      </c>
       <c r="F80" s="2" t="s">
         <v>5814</v>
       </c>
@@ -50214,7 +51195,7 @@
         <v>5814</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>5815</v>
       </c>
@@ -50224,6 +51205,12 @@
       <c r="C81" t="s">
         <v>1112</v>
       </c>
+      <c r="D81" s="12" t="s">
+        <v>12036</v>
+      </c>
+      <c r="E81" s="12" t="s">
+        <v>12113</v>
+      </c>
       <c r="F81" s="2" t="s">
         <v>6824</v>
       </c>
@@ -50243,7 +51230,7 @@
         <v>6210</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>5817</v>
       </c>
@@ -50253,6 +51240,12 @@
       <c r="C82" t="s">
         <v>7171</v>
       </c>
+      <c r="D82" s="12" t="s">
+        <v>12037</v>
+      </c>
+      <c r="E82" s="12" t="s">
+        <v>12037</v>
+      </c>
       <c r="F82" s="2" t="s">
         <v>5818</v>
       </c>
@@ -50272,7 +51265,7 @@
         <v>6211</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>5819</v>
       </c>
@@ -50282,6 +51275,12 @@
       <c r="C83" t="s">
         <v>7172</v>
       </c>
+      <c r="D83" s="12" t="s">
+        <v>12038</v>
+      </c>
+      <c r="E83" s="12" t="s">
+        <v>12038</v>
+      </c>
       <c r="F83" s="2" t="s">
         <v>6825</v>
       </c>
@@ -50301,7 +51300,7 @@
         <v>11481</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>5820</v>
       </c>
@@ -50311,6 +51310,12 @@
       <c r="C84" t="s">
         <v>7173</v>
       </c>
+      <c r="D84" s="12" t="s">
+        <v>12039</v>
+      </c>
+      <c r="E84" s="12" t="s">
+        <v>12039</v>
+      </c>
       <c r="F84" s="2" t="s">
         <v>6826</v>
       </c>
@@ -50330,7 +51335,7 @@
         <v>11482</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>5821</v>
       </c>
@@ -50340,6 +51345,12 @@
       <c r="C85" t="s">
         <v>7174</v>
       </c>
+      <c r="D85" s="12" t="s">
+        <v>12040</v>
+      </c>
+      <c r="E85" s="12" t="s">
+        <v>12040</v>
+      </c>
       <c r="F85" s="2" t="s">
         <v>6827</v>
       </c>
@@ -50359,7 +51370,7 @@
         <v>6214</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>5823</v>
       </c>
@@ -50369,6 +51380,12 @@
       <c r="C86" t="s">
         <v>7175</v>
       </c>
+      <c r="D86" s="12" t="s">
+        <v>12041</v>
+      </c>
+      <c r="E86" s="12" t="s">
+        <v>12114</v>
+      </c>
       <c r="F86" s="2" t="s">
         <v>5824</v>
       </c>
@@ -50388,7 +51405,7 @@
         <v>11483</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>5825</v>
       </c>
@@ -50398,6 +51415,12 @@
       <c r="C87" t="s">
         <v>7176</v>
       </c>
+      <c r="D87" s="12" t="s">
+        <v>12042</v>
+      </c>
+      <c r="E87" s="12" t="s">
+        <v>12115</v>
+      </c>
       <c r="F87" s="2" t="s">
         <v>6828</v>
       </c>
@@ -50417,7 +51440,7 @@
         <v>11484</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>5827</v>
       </c>
@@ -50427,6 +51450,12 @@
       <c r="C88" t="s">
         <v>7177</v>
       </c>
+      <c r="D88" s="12" t="s">
+        <v>12043</v>
+      </c>
+      <c r="E88" s="12" t="s">
+        <v>12043</v>
+      </c>
       <c r="F88" s="2" t="s">
         <v>5828</v>
       </c>
@@ -50446,7 +51475,7 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>5829</v>
       </c>
@@ -50456,6 +51485,12 @@
       <c r="C89" t="s">
         <v>7178</v>
       </c>
+      <c r="D89" s="12" t="s">
+        <v>12044</v>
+      </c>
+      <c r="E89" s="12" t="s">
+        <v>12116</v>
+      </c>
       <c r="F89" s="2" t="s">
         <v>6829</v>
       </c>
@@ -50475,7 +51510,7 @@
         <v>6217</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>5831</v>
       </c>
@@ -50485,6 +51520,12 @@
       <c r="C90" t="s">
         <v>7179</v>
       </c>
+      <c r="D90" s="12" t="s">
+        <v>12045</v>
+      </c>
+      <c r="E90" s="12" t="s">
+        <v>12045</v>
+      </c>
       <c r="F90" s="2" t="s">
         <v>5832</v>
       </c>
@@ -50504,7 +51545,7 @@
         <v>5832</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>5833</v>
       </c>
@@ -50514,6 +51555,12 @@
       <c r="C91" t="s">
         <v>7180</v>
       </c>
+      <c r="D91" s="12" t="s">
+        <v>12046</v>
+      </c>
+      <c r="E91" s="12" t="s">
+        <v>12117</v>
+      </c>
       <c r="F91" s="2" t="s">
         <v>5834</v>
       </c>
@@ -50533,7 +51580,7 @@
         <v>5834</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>5835</v>
       </c>
@@ -50543,6 +51590,12 @@
       <c r="C92" t="s">
         <v>7181</v>
       </c>
+      <c r="D92" s="12" t="s">
+        <v>12047</v>
+      </c>
+      <c r="E92" s="12" t="s">
+        <v>12047</v>
+      </c>
       <c r="F92" s="2" t="s">
         <v>5836</v>
       </c>
@@ -50562,7 +51615,7 @@
         <v>2609</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>5837</v>
       </c>
@@ -50572,6 +51625,12 @@
       <c r="C93" t="s">
         <v>7182</v>
       </c>
+      <c r="D93" s="12" t="s">
+        <v>12048</v>
+      </c>
+      <c r="E93" s="12" t="s">
+        <v>12118</v>
+      </c>
       <c r="F93" s="2" t="s">
         <v>5838</v>
       </c>
@@ -50591,7 +51650,7 @@
         <v>5838</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>5839</v>
       </c>
@@ -50601,6 +51660,12 @@
       <c r="C94" t="s">
         <v>5840</v>
       </c>
+      <c r="D94" s="12" t="s">
+        <v>12049</v>
+      </c>
+      <c r="E94" s="12" t="s">
+        <v>12119</v>
+      </c>
       <c r="F94" s="2" t="s">
         <v>5840</v>
       </c>
@@ -50620,7 +51685,7 @@
         <v>5840</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>5841</v>
       </c>
@@ -50630,6 +51695,12 @@
       <c r="C95" t="s">
         <v>5842</v>
       </c>
+      <c r="D95" s="12" t="s">
+        <v>12050</v>
+      </c>
+      <c r="E95" s="12" t="s">
+        <v>12120</v>
+      </c>
       <c r="F95" s="2" t="s">
         <v>5842</v>
       </c>
@@ -50649,7 +51720,7 @@
         <v>11485</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>5843</v>
       </c>
@@ -50659,6 +51730,12 @@
       <c r="C96" t="s">
         <v>7183</v>
       </c>
+      <c r="D96" s="12" t="s">
+        <v>12051</v>
+      </c>
+      <c r="E96" s="12" t="s">
+        <v>12121</v>
+      </c>
       <c r="F96" s="2" t="s">
         <v>5844</v>
       </c>
@@ -50678,7 +51755,7 @@
         <v>11486</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>5845</v>
       </c>
@@ -50688,6 +51765,12 @@
       <c r="C97" t="s">
         <v>7184</v>
       </c>
+      <c r="D97" s="12" t="s">
+        <v>12052</v>
+      </c>
+      <c r="E97" s="12" t="s">
+        <v>12122</v>
+      </c>
       <c r="F97" s="2" t="s">
         <v>5846</v>
       </c>
@@ -50707,7 +51790,7 @@
         <v>6222</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>5847</v>
       </c>
@@ -50717,6 +51800,12 @@
       <c r="C98" t="s">
         <v>7185</v>
       </c>
+      <c r="D98" s="12" t="s">
+        <v>12053</v>
+      </c>
+      <c r="E98" s="12" t="s">
+        <v>12123</v>
+      </c>
       <c r="F98" s="2" t="s">
         <v>5848</v>
       </c>
@@ -50736,7 +51825,7 @@
         <v>5848</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>5849</v>
       </c>
@@ -50746,6 +51835,12 @@
       <c r="C99" t="s">
         <v>7186</v>
       </c>
+      <c r="D99" s="12" t="s">
+        <v>12054</v>
+      </c>
+      <c r="E99" s="12" t="s">
+        <v>12124</v>
+      </c>
       <c r="F99" s="2" t="s">
         <v>5850</v>
       </c>
@@ -50765,7 +51860,7 @@
         <v>5850</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>5851</v>
       </c>
@@ -50775,6 +51870,12 @@
       <c r="C100" t="s">
         <v>5852</v>
       </c>
+      <c r="D100" s="12" t="s">
+        <v>12055</v>
+      </c>
+      <c r="E100" s="12" t="s">
+        <v>12125</v>
+      </c>
       <c r="F100" s="2" t="s">
         <v>5852</v>
       </c>
@@ -50794,7 +51895,7 @@
         <v>5852</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>5853</v>
       </c>
@@ -50804,6 +51905,12 @@
       <c r="C101" t="s">
         <v>7187</v>
       </c>
+      <c r="D101" s="12" t="s">
+        <v>12056</v>
+      </c>
+      <c r="E101" s="12" t="s">
+        <v>12126</v>
+      </c>
       <c r="F101" s="2" t="s">
         <v>5854</v>
       </c>
@@ -50823,7 +51930,7 @@
         <v>5854</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>5855</v>
       </c>
@@ -50833,6 +51940,12 @@
       <c r="C102" t="s">
         <v>7188</v>
       </c>
+      <c r="D102" s="12" t="s">
+        <v>12057</v>
+      </c>
+      <c r="E102" s="12" t="s">
+        <v>12127</v>
+      </c>
       <c r="F102" s="2" t="s">
         <v>5856</v>
       </c>
@@ -50852,7 +51965,7 @@
         <v>5856</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>5857</v>
       </c>
@@ -50862,6 +51975,12 @@
       <c r="C103" t="s">
         <v>7189</v>
       </c>
+      <c r="D103" s="12" t="s">
+        <v>12058</v>
+      </c>
+      <c r="E103" s="12" t="s">
+        <v>12128</v>
+      </c>
       <c r="F103" s="2" t="s">
         <v>5858</v>
       </c>
@@ -50881,7 +52000,7 @@
         <v>5858</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>5859</v>
       </c>
@@ -50891,6 +52010,12 @@
       <c r="C104" t="s">
         <v>7190</v>
       </c>
+      <c r="D104" s="12" t="s">
+        <v>12059</v>
+      </c>
+      <c r="E104" s="12" t="s">
+        <v>12129</v>
+      </c>
       <c r="F104" s="2" t="s">
         <v>5860</v>
       </c>
@@ -50910,7 +52035,7 @@
         <v>11487</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>11940</v>
       </c>
@@ -50920,6 +52045,12 @@
       <c r="C105" t="s">
         <v>7191</v>
       </c>
+      <c r="D105" s="12" t="s">
+        <v>12060</v>
+      </c>
+      <c r="E105" s="12" t="s">
+        <v>12060</v>
+      </c>
       <c r="F105" s="2" t="s">
         <v>6830</v>
       </c>
@@ -50939,7 +52070,7 @@
         <v>11488</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>11941</v>
       </c>
@@ -50949,6 +52080,12 @@
       <c r="C106" t="s">
         <v>7192</v>
       </c>
+      <c r="D106" s="12" t="s">
+        <v>12061</v>
+      </c>
+      <c r="E106" s="12" t="s">
+        <v>12130</v>
+      </c>
       <c r="F106" s="2" t="s">
         <v>6831</v>
       </c>
@@ -50968,7 +52105,7 @@
         <v>11489</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>11942</v>
       </c>
@@ -50978,6 +52115,12 @@
       <c r="C107" t="s">
         <v>7193</v>
       </c>
+      <c r="D107" s="12" t="s">
+        <v>12062</v>
+      </c>
+      <c r="E107" s="12" t="s">
+        <v>12131</v>
+      </c>
       <c r="F107" s="2" t="s">
         <v>6832</v>
       </c>
@@ -50997,7 +52140,7 @@
         <v>11490</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>11943</v>
       </c>
@@ -51007,6 +52150,12 @@
       <c r="C108" t="s">
         <v>5864</v>
       </c>
+      <c r="D108" s="12" t="s">
+        <v>12063</v>
+      </c>
+      <c r="E108" s="12" t="s">
+        <v>12132</v>
+      </c>
       <c r="F108" s="2" t="s">
         <v>5864</v>
       </c>
@@ -51026,7 +52175,7 @@
         <v>5864</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>11944</v>
       </c>
@@ -51036,6 +52185,12 @@
       <c r="C109" t="s">
         <v>7194</v>
       </c>
+      <c r="D109" s="12" t="s">
+        <v>12064</v>
+      </c>
+      <c r="E109" s="12" t="s">
+        <v>12133</v>
+      </c>
       <c r="F109" s="2" t="s">
         <v>6833</v>
       </c>
@@ -51055,7 +52210,7 @@
         <v>11491</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>11945</v>
       </c>
@@ -51065,6 +52220,12 @@
       <c r="C110" t="s">
         <v>7195</v>
       </c>
+      <c r="D110" s="12" t="s">
+        <v>12065</v>
+      </c>
+      <c r="E110" s="12" t="s">
+        <v>12065</v>
+      </c>
       <c r="F110" s="2" t="s">
         <v>5866</v>
       </c>
@@ -51084,7 +52245,7 @@
         <v>5866</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>11946</v>
       </c>
@@ -51094,6 +52255,12 @@
       <c r="C111" t="s">
         <v>7196</v>
       </c>
+      <c r="D111" s="12" t="s">
+        <v>12066</v>
+      </c>
+      <c r="E111" s="12" t="s">
+        <v>12134</v>
+      </c>
       <c r="F111" s="2" t="s">
         <v>5867</v>
       </c>
@@ -51113,7 +52280,7 @@
         <v>5867</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>11947</v>
       </c>
@@ -51123,6 +52290,12 @@
       <c r="C112" t="s">
         <v>7197</v>
       </c>
+      <c r="D112" s="12" t="s">
+        <v>12067</v>
+      </c>
+      <c r="E112" s="12" t="s">
+        <v>12135</v>
+      </c>
       <c r="F112" s="2" t="s">
         <v>5868</v>
       </c>
@@ -51142,7 +52315,7 @@
         <v>5868</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>11948</v>
       </c>
@@ -51152,6 +52325,12 @@
       <c r="C113" t="s">
         <v>7198</v>
       </c>
+      <c r="D113" s="12" t="s">
+        <v>12068</v>
+      </c>
+      <c r="E113" s="12" t="s">
+        <v>12136</v>
+      </c>
       <c r="F113" s="2" t="s">
         <v>5869</v>
       </c>
@@ -51171,7 +52350,7 @@
         <v>11492</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>11949</v>
       </c>
@@ -51181,6 +52360,12 @@
       <c r="C114" t="s">
         <v>7199</v>
       </c>
+      <c r="D114" s="12" t="s">
+        <v>12069</v>
+      </c>
+      <c r="E114" s="12" t="s">
+        <v>12069</v>
+      </c>
       <c r="F114" s="2" t="s">
         <v>5870</v>
       </c>
@@ -51200,7 +52385,7 @@
         <v>5870</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>11950</v>
       </c>
@@ -51210,6 +52395,12 @@
       <c r="C115" t="s">
         <v>7200</v>
       </c>
+      <c r="D115" s="12" t="s">
+        <v>12070</v>
+      </c>
+      <c r="E115" s="12" t="s">
+        <v>12070</v>
+      </c>
       <c r="F115" s="2" t="s">
         <v>5871</v>
       </c>
@@ -51229,7 +52420,7 @@
         <v>5871</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>11951</v>
       </c>
@@ -51239,6 +52430,12 @@
       <c r="C116" t="s">
         <v>7201</v>
       </c>
+      <c r="D116" s="12" t="s">
+        <v>12071</v>
+      </c>
+      <c r="E116" s="12" t="s">
+        <v>12137</v>
+      </c>
       <c r="F116" s="2" t="s">
         <v>6834</v>
       </c>
@@ -51258,7 +52455,7 @@
         <v>11493</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>11952</v>
       </c>
@@ -51268,6 +52465,12 @@
       <c r="C117" t="s">
         <v>7202</v>
       </c>
+      <c r="D117" s="12" t="s">
+        <v>12072</v>
+      </c>
+      <c r="E117" s="12" t="s">
+        <v>12138</v>
+      </c>
       <c r="F117" s="2" t="s">
         <v>5873</v>
       </c>
@@ -51287,7 +52490,7 @@
         <v>5873</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>11953</v>
       </c>
@@ -51297,6 +52500,12 @@
       <c r="C118" t="s">
         <v>7203</v>
       </c>
+      <c r="D118" s="12" t="s">
+        <v>12073</v>
+      </c>
+      <c r="E118" s="12" t="s">
+        <v>12139</v>
+      </c>
       <c r="F118" s="2" t="s">
         <v>5874</v>
       </c>
@@ -51316,7 +52525,7 @@
         <v>5874</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>11954</v>
       </c>
@@ -51326,6 +52535,12 @@
       <c r="C119" t="s">
         <v>7204</v>
       </c>
+      <c r="D119" s="12" t="s">
+        <v>12074</v>
+      </c>
+      <c r="E119" s="12" t="s">
+        <v>12140</v>
+      </c>
       <c r="F119" s="2" t="s">
         <v>6835</v>
       </c>
@@ -51345,7 +52560,7 @@
         <v>11494</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>11955</v>
       </c>
@@ -51355,6 +52570,12 @@
       <c r="C120" t="s">
         <v>5876</v>
       </c>
+      <c r="D120" s="12" t="s">
+        <v>12075</v>
+      </c>
+      <c r="E120" s="12" t="s">
+        <v>12075</v>
+      </c>
       <c r="F120" s="2" t="s">
         <v>5876</v>
       </c>
@@ -51374,7 +52595,7 @@
         <v>5876</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>11956</v>
       </c>
@@ -51384,6 +52605,12 @@
       <c r="C121" t="s">
         <v>7205</v>
       </c>
+      <c r="D121" s="12" t="s">
+        <v>12076</v>
+      </c>
+      <c r="E121" s="12" t="s">
+        <v>12076</v>
+      </c>
       <c r="F121" s="2" t="s">
         <v>5877</v>
       </c>
@@ -51403,7 +52630,7 @@
         <v>6230</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>11957</v>
       </c>
@@ -51413,6 +52640,12 @@
       <c r="C122" t="s">
         <v>7206</v>
       </c>
+      <c r="D122" s="12" t="s">
+        <v>12077</v>
+      </c>
+      <c r="E122" s="12" t="s">
+        <v>12141</v>
+      </c>
       <c r="F122" s="2" t="s">
         <v>5878</v>
       </c>
@@ -51432,7 +52665,7 @@
         <v>5878</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>11958</v>
       </c>
@@ -51441,6 +52674,12 @@
       </c>
       <c r="C123" t="s">
         <v>7207</v>
+      </c>
+      <c r="D123" s="12" t="s">
+        <v>12078</v>
+      </c>
+      <c r="E123" s="12" t="s">
+        <v>12142</v>
       </c>
       <c r="F123" s="2" t="s">
         <v>5879</v>
@@ -53350,7 +54589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBBA198A-82A8-4E0B-B616-B0C234568614}">
   <dimension ref="A1:O79"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A45" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -55826,7 +57065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607EE55B-01B9-43A2-ABDF-547288CE50DD}">
   <dimension ref="A1:O95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
@@ -59089,7 +60328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8757A3A2-1687-42DC-847A-464A3A95A6DE}">
   <dimension ref="A1:O175"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A141" workbookViewId="0">
       <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
@@ -65245,7 +66484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ADBB5F6-192B-4660-A6DC-9C225D90B84F}">
   <dimension ref="A1:O399"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A365" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
@@ -79300,7 +80539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F90AF4D-9877-467E-81BF-A9F8CCE99B88}">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>

</xml_diff>